<commit_message>
fix name error in perf report generation (#421)
Closes issue `https://github.com/AMD-AGI/TraceLens/issues/418`

<!--
Copyright (c) 2024 - 2025 Advanced Micro Devices, Inc. All rights
reserved.

See LICENSE for license information.
-->

---------

Co-authored-by: Copilot <175728472+Copilot@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/tests/traces/mi300/jax_conv_minimal_perf_report.xlsx
+++ b/tests/traces/mi300/jax_conv_minimal_perf_report.xlsx
@@ -13,10 +13,9 @@
     <sheet name="kernel_launchers_summary" sheetId="4" state="visible" r:id="rId4"/>
     <sheet name="kernel_launchers_summary_by_category" sheetId="5" state="visible" r:id="rId5"/>
     <sheet name="kernel_launchers_unique_args" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="xla_summary" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet name="op_jax_gemm" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet name="op_jax_conv" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet name="op_jax_te" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="df_xla_perf" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="xla_summary" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="op_conv" sheetId="9" state="visible" r:id="rId9"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -725,24 +724,6 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
@@ -889,7 +870,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L26"/>
+  <dimension ref="A1:M26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -958,6 +939,11 @@
           <t>kernel_details</t>
         </is>
       </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>GPU_kernel_launch_latency</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -1010,6 +996,9 @@
           <t>[{'name': 'loop_transpose_fusion', 'dur': 6.89, 'custom_call_target': 'NA', 'operands': ['bf16[1,2,2,16,5120]{4,3,2,1,0}'], 'outputs': 'NA', 'metadata': 'metadata={op_name="kernel"'}]</t>
         </is>
       </c>
+      <c r="M2" t="n">
+        <v>20.94200000003912</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -1062,6 +1051,9 @@
           <t>[{'name': 'input_transpose_fusion_1', 'dur': 42.983, 'custom_call_target': 'NA', 'operands': ['bf16[1,32,60,104,16]{4,3,2,1,0}'], 'outputs': 'NA', 'metadata': 'metadata={op_name="x"'}]</t>
         </is>
       </c>
+      <c r="M3" t="n">
+        <v>12.1589999999851</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -1114,6 +1106,9 @@
           <t>[{'name': 'Im3d2Col', 'dur': 16.104, 'custom_call_target': 'custom_call_target="__cudnn$convForward"', 'operands': ['bf16[1,16,32,60,104]{4,3,2,1,0}', 'bf16[5120,16,1,2,2]{4,3,2,1,0}'], 'outputs': 'NA', 'metadata': 'metadata={op_name="jit(forward_3d_conv)/jit(main)/conv_general_dilated" source_file="/workspace/conv-jax/jax_conv_profiling.py" source_line=77'}]</t>
         </is>
       </c>
+      <c r="M4" t="n">
+        <v>16.84600000013597</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -1166,6 +1161,9 @@
           <t>[{'name': 'Cijk_Ailk_Bljk_BBS_BH_MT256x128x64_MI16x16x16x1_SN_1LDSB0_APM1_ABV0_ACED0_AF0EM1_AF1EM1_AMAS3_ASE_ASGT_ASLT_ASM_ASAE01_ASCE01_ASEM1_AAC0_BL1_BS1_CLR1_DTLA0_DTLB0_DTVA1_DTVB0_DVO0_ETSP_EPS1_ELFLR0_EMLL0_FSSC10_FL0_GLVWA2_GLVWB4_GRCGA1_GRCGB1_GRPM1_GRVWn1_GSU1_GSUASB_GLS0_ISA942_IU1_K1_KLA_LBSPPA0_LBSPPB1024_LPA0_LPB4_LDL1_LRVW4_LWPMn1_LDW0_FMA_MIAV0_MDA2_MO40_MMFSC_MKFGSU256_NTA0_NTB0_NTC0_NTD0_NEPBS0_NLCA2_NLCB2_ONLL1_OPLV0_PK0_PAP0_PGR2_PLR5_PKA0_SIA3_SLW1_SS1_SU8_SUM0_SUS256_SCIUI1_SPO1_SRVW0_SSO0_SVW2_SNLL0_TSGRA0_TSGRB0_TT4_128_TLDS0_UMLDSA0_UMLDSB0_U64SL1_USFGROn1_VAW1_VSn1_VW2_VWB4_VFLRP1_WSGRA0_WSGRB0_WS64_WG64_4_1_WGM1', 'dur': 291.19, 'custom_call_target': 'custom_call_target="__cudnn$convForward"', 'operands': ['bf16[1,16,32,60,104]{4,3,2,1,0}', 'bf16[5120,16,1,2,2]{4,3,2,1,0}'], 'outputs': 'NA', 'metadata': 'metadata={op_name="jit(forward_3d_conv)/jit(main)/conv_general_dilated" source_file="/workspace/conv-jax/jax_conv_profiling.py" source_line=77'}]</t>
         </is>
       </c>
+      <c r="M5" t="n">
+        <v>15.73399999993853</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -1218,6 +1216,9 @@
           <t>[{'name': 'input_transpose_fusion', 'dur': 475.582, 'custom_call_target': 'NA', 'operands': ['bf16[1,5120,34,31,53]{4,3,2,1,0}'], 'outputs': 'NA', 'metadata': 'metadata={op_name="jit(forward_3d_conv)/jit(main)/conv_general_dilated" source_file="/workspace/conv-jax/jax_conv_profiling.py" source_line=77'}]</t>
         </is>
       </c>
+      <c r="M6" t="n">
+        <v>294.3659999999218</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -1270,6 +1271,9 @@
           <t>[{'name': 'loop_transpose_fusion', 'dur': 5.048, 'custom_call_target': 'NA', 'operands': ['bf16[1,2,2,16,5120]{4,3,2,1,0}'], 'outputs': 'NA', 'metadata': 'metadata={op_name="kernel"'}]</t>
         </is>
       </c>
+      <c r="M7" t="n">
+        <v>14.40200000000186</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -1322,6 +1326,9 @@
           <t>[{'name': 'input_transpose_fusion_1', 'dur': 6.689, 'custom_call_target': 'NA', 'operands': ['bf16[1,32,60,104,16]{4,3,2,1,0}'], 'outputs': 'NA', 'metadata': 'metadata={op_name="x"'}]</t>
         </is>
       </c>
+      <c r="M8" t="n">
+        <v>10.92700000014156</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1374,6 +1381,9 @@
           <t>[{'name': 'Im3d2Col', 'dur': 16.144, 'custom_call_target': 'custom_call_target="__cudnn$convForward"', 'operands': ['bf16[1,16,32,60,104]{4,3,2,1,0}', 'bf16[5120,16,1,2,2]{4,3,2,1,0}'], 'outputs': 'NA', 'metadata': 'metadata={op_name="jit(forward_3d_conv)/jit(main)/conv_general_dilated" source_file="/workspace/conv-jax/jax_conv_profiling.py" source_line=77'}]</t>
         </is>
       </c>
+      <c r="M9" t="n">
+        <v>14.7019999998156</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1426,6 +1436,9 @@
           <t>[{'name': 'Cijk_Ailk_Bljk_BBS_BH_MT256x128x64_MI16x16x16x1_SN_1LDSB0_APM1_ABV0_ACED0_AF0EM1_AF1EM1_AMAS3_ASE_ASGT_ASLT_ASM_ASAE01_ASCE01_ASEM1_AAC0_BL1_BS1_CLR1_DTLA0_DTLB0_DTVA1_DTVB0_DVO0_ETSP_EPS1_ELFLR0_EMLL0_FSSC10_FL0_GLVWA2_GLVWB4_GRCGA1_GRCGB1_GRPM1_GRVWn1_GSU1_GSUASB_GLS0_ISA942_IU1_K1_KLA_LBSPPA0_LBSPPB1024_LPA0_LPB4_LDL1_LRVW4_LWPMn1_LDW0_FMA_MIAV0_MDA2_MO40_MMFSC_MKFGSU256_NTA0_NTB0_NTC0_NTD0_NEPBS0_NLCA2_NLCB2_ONLL1_OPLV0_PK0_PAP0_PGR2_PLR5_PKA0_SIA3_SLW1_SS1_SU8_SUM0_SUS256_SCIUI1_SPO1_SRVW0_SSO0_SVW2_SNLL0_TSGRA0_TSGRB0_TT4_128_TLDS0_UMLDSA0_UMLDSB0_U64SL1_USFGROn1_VAW1_VSn1_VW2_VWB4_VFLRP1_WSGRA0_WSGRB0_WS64_WG64_4_1_WGM1', 'dur': 292.752, 'custom_call_target': 'custom_call_target="__cudnn$convForward"', 'operands': ['bf16[1,16,32,60,104]{4,3,2,1,0}', 'bf16[5120,16,1,2,2]{4,3,2,1,0}'], 'outputs': 'NA', 'metadata': 'metadata={op_name="jit(forward_3d_conv)/jit(main)/conv_general_dilated" source_file="/workspace/conv-jax/jax_conv_profiling.py" source_line=77'}]</t>
         </is>
       </c>
+      <c r="M10" t="n">
+        <v>13.06099999998696</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1478,6 +1491,9 @@
           <t>[{'name': 'input_transpose_fusion', 'dur': 366.06, 'custom_call_target': 'NA', 'operands': ['bf16[1,5120,34,31,53]{4,3,2,1,0}'], 'outputs': 'NA', 'metadata': 'metadata={op_name="jit(forward_3d_conv)/jit(main)/conv_general_dilated" source_file="/workspace/conv-jax/jax_conv_profiling.py" source_line=77'}]</t>
         </is>
       </c>
+      <c r="M11" t="n">
+        <v>295.3469999998342</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -1530,6 +1546,9 @@
           <t>[{'name': 'loop_transpose_fusion', 'dur': 4.807, 'custom_call_target': 'NA', 'operands': ['bf16[1,2,2,16,5120]{4,3,2,1,0}'], 'outputs': 'NA', 'metadata': 'metadata={op_name="kernel"'}]</t>
         </is>
       </c>
+      <c r="M12" t="n">
+        <v>14.72200000006706</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -1582,6 +1601,9 @@
           <t>[{'name': 'input_transpose_fusion_1', 'dur': 6.53, 'custom_call_target': 'NA', 'operands': ['bf16[1,32,60,104,16]{4,3,2,1,0}'], 'outputs': 'NA', 'metadata': 'metadata={op_name="x"'}]</t>
         </is>
       </c>
+      <c r="M13" t="n">
+        <v>11.14699999988079</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -1634,6 +1656,9 @@
           <t>[{'name': 'Im3d2Col', 'dur': 16.264, 'custom_call_target': 'custom_call_target="__cudnn$convForward"', 'operands': ['bf16[1,16,32,60,104]{4,3,2,1,0}', 'bf16[5120,16,1,2,2]{4,3,2,1,0}'], 'outputs': 'NA', 'metadata': 'metadata={op_name="jit(forward_3d_conv)/jit(main)/conv_general_dilated" source_file="/workspace/conv-jax/jax_conv_profiling.py" source_line=77'}]</t>
         </is>
       </c>
+      <c r="M14" t="n">
+        <v>13.55099999997765</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1686,6 +1711,9 @@
           <t>[{'name': 'Cijk_Ailk_Bljk_BBS_BH_MT256x128x64_MI16x16x16x1_SN_1LDSB0_APM1_ABV0_ACED0_AF0EM1_AF1EM1_AMAS3_ASE_ASGT_ASLT_ASM_ASAE01_ASCE01_ASEM1_AAC0_BL1_BS1_CLR1_DTLA0_DTLB0_DTVA1_DTVB0_DVO0_ETSP_EPS1_ELFLR0_EMLL0_FSSC10_FL0_GLVWA2_GLVWB4_GRCGA1_GRCGB1_GRPM1_GRVWn1_GSU1_GSUASB_GLS0_ISA942_IU1_K1_KLA_LBSPPA0_LBSPPB1024_LPA0_LPB4_LDL1_LRVW4_LWPMn1_LDW0_FMA_MIAV0_MDA2_MO40_MMFSC_MKFGSU256_NTA0_NTB0_NTC0_NTD0_NEPBS0_NLCA2_NLCB2_ONLL1_OPLV0_PK0_PAP0_PGR2_PLR5_PKA0_SIA3_SLW1_SS1_SU8_SUM0_SUS256_SCIUI1_SPO1_SRVW0_SSO0_SVW2_SNLL0_TSGRA0_TSGRB0_TT4_128_TLDS0_UMLDSA0_UMLDSB0_U64SL1_USFGROn1_VAW1_VSn1_VW2_VWB4_VFLRP1_WSGRA0_WSGRB0_WS64_WG64_4_1_WGM1', 'dur': 288.466, 'custom_call_target': 'custom_call_target="__cudnn$convForward"', 'operands': ['bf16[1,16,32,60,104]{4,3,2,1,0}', 'bf16[5120,16,1,2,2]{4,3,2,1,0}'], 'outputs': 'NA', 'metadata': 'metadata={op_name="jit(forward_3d_conv)/jit(main)/conv_general_dilated" source_file="/workspace/conv-jax/jax_conv_profiling.py" source_line=77'}]</t>
         </is>
       </c>
+      <c r="M15" t="n">
+        <v>8.503000000026077</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1738,6 +1766,9 @@
           <t>[{'name': 'input_transpose_fusion', 'dur': 370.347, 'custom_call_target': 'NA', 'operands': ['bf16[1,5120,34,31,53]{4,3,2,1,0}'], 'outputs': 'NA', 'metadata': 'metadata={op_name="jit(forward_3d_conv)/jit(main)/conv_general_dilated" source_file="/workspace/conv-jax/jax_conv_profiling.py" source_line=77'}]</t>
         </is>
       </c>
+      <c r="M16" t="n">
+        <v>287.7750000001397</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -1790,6 +1821,9 @@
           <t>[{'name': 'loop_transpose_fusion', 'dur': 4.968, 'custom_call_target': 'NA', 'operands': ['bf16[1,2,2,16,5120]{4,3,2,1,0}'], 'outputs': 'NA', 'metadata': 'metadata={op_name="kernel"'}]</t>
         </is>
       </c>
+      <c r="M17" t="n">
+        <v>21.33199999993667</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1842,6 +1876,9 @@
           <t>[{'name': 'input_transpose_fusion_1', 'dur': 6.329, 'custom_call_target': 'NA', 'operands': ['bf16[1,32,60,104,16]{4,3,2,1,0}'], 'outputs': 'NA', 'metadata': 'metadata={op_name="x"'}]</t>
         </is>
       </c>
+      <c r="M18" t="n">
+        <v>9.385000000009313</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -1894,6 +1931,9 @@
           <t>[{'name': 'Im3d2Col', 'dur': 16.143, 'custom_call_target': 'custom_call_target="__cudnn$convForward"', 'operands': ['bf16[1,16,32,60,104]{4,3,2,1,0}', 'bf16[5120,16,1,2,2]{4,3,2,1,0}'], 'outputs': 'NA', 'metadata': 'metadata={op_name="jit(forward_3d_conv)/jit(main)/conv_general_dilated" source_file="/workspace/conv-jax/jax_conv_profiling.py" source_line=77'}]</t>
         </is>
       </c>
+      <c r="M19" t="n">
+        <v>14.77299999981187</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1946,6 +1986,9 @@
           <t>[{'name': 'Cijk_Ailk_Bljk_BBS_BH_MT256x128x64_MI16x16x16x1_SN_1LDSB0_APM1_ABV0_ACED0_AF0EM1_AF1EM1_AMAS3_ASE_ASGT_ASLT_ASM_ASAE01_ASCE01_ASEM1_AAC0_BL1_BS1_CLR1_DTLA0_DTLB0_DTVA1_DTVB0_DVO0_ETSP_EPS1_ELFLR0_EMLL0_FSSC10_FL0_GLVWA2_GLVWB4_GRCGA1_GRCGB1_GRPM1_GRVWn1_GSU1_GSUASB_GLS0_ISA942_IU1_K1_KLA_LBSPPA0_LBSPPB1024_LPA0_LPB4_LDL1_LRVW4_LWPMn1_LDW0_FMA_MIAV0_MDA2_MO40_MMFSC_MKFGSU256_NTA0_NTB0_NTC0_NTD0_NEPBS0_NLCA2_NLCB2_ONLL1_OPLV0_PK0_PAP0_PGR2_PLR5_PKA0_SIA3_SLW1_SS1_SU8_SUM0_SUS256_SCIUI1_SPO1_SRVW0_SSO0_SVW2_SNLL0_TSGRA0_TSGRB0_TT4_128_TLDS0_UMLDSA0_UMLDSB0_U64SL1_USFGROn1_VAW1_VSn1_VW2_VWB4_VFLRP1_WSGRA0_WSGRB0_WS64_WG64_4_1_WGM1', 'dur': 293.593, 'custom_call_target': 'custom_call_target="__cudnn$convForward"', 'operands': ['bf16[1,16,32,60,104]{4,3,2,1,0}', 'bf16[5120,16,1,2,2]{4,3,2,1,0}'], 'outputs': 'NA', 'metadata': 'metadata={op_name="jit(forward_3d_conv)/jit(main)/conv_general_dilated" source_file="/workspace/conv-jax/jax_conv_profiling.py" source_line=77'}]</t>
         </is>
       </c>
+      <c r="M20" t="n">
+        <v>9.545000000158325</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -1998,6 +2041,9 @@
           <t>[{'name': 'input_transpose_fusion', 'dur': 369.426, 'custom_call_target': 'NA', 'operands': ['bf16[1,5120,34,31,53]{4,3,2,1,0}'], 'outputs': 'NA', 'metadata': 'metadata={op_name="jit(forward_3d_conv)/jit(main)/conv_general_dilated" source_file="/workspace/conv-jax/jax_conv_profiling.py" source_line=77'}]</t>
         </is>
       </c>
+      <c r="M21" t="n">
+        <v>293.1029999998864</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -2050,6 +2096,9 @@
           <t>[{'name': 'loop_transpose_fusion', 'dur': 4.727, 'custom_call_target': 'NA', 'operands': ['bf16[1,2,2,16,5120]{4,3,2,1,0}'], 'outputs': 'NA', 'metadata': 'metadata={op_name="kernel"'}]</t>
         </is>
       </c>
+      <c r="M22" t="n">
+        <v>15.06200000015087</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -2102,6 +2151,9 @@
           <t>[{'name': 'input_transpose_fusion_1', 'dur': 6.73, 'custom_call_target': 'NA', 'operands': ['bf16[1,32,60,104,16]{4,3,2,1,0}'], 'outputs': 'NA', 'metadata': 'metadata={op_name="x"'}]</t>
         </is>
       </c>
+      <c r="M23" t="n">
+        <v>11.5570000000298</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -2154,6 +2206,9 @@
           <t>[{'name': 'Im3d2Col', 'dur': 16.424, 'custom_call_target': 'custom_call_target="__cudnn$convForward"', 'operands': ['bf16[1,16,32,60,104]{4,3,2,1,0}', 'bf16[5120,16,1,2,2]{4,3,2,1,0}'], 'outputs': 'NA', 'metadata': 'metadata={op_name="jit(forward_3d_conv)/jit(main)/conv_general_dilated" source_file="/workspace/conv-jax/jax_conv_profiling.py" source_line=77'}]</t>
         </is>
       </c>
+      <c r="M24" t="n">
+        <v>14.02099999994971</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -2206,6 +2261,9 @@
           <t>[{'name': 'Cijk_Ailk_Bljk_BBS_BH_MT256x128x64_MI16x16x16x1_SN_1LDSB0_APM1_ABV0_ACED0_AF0EM1_AF1EM1_AMAS3_ASE_ASGT_ASLT_ASM_ASAE01_ASCE01_ASEM1_AAC0_BL1_BS1_CLR1_DTLA0_DTLB0_DTVA1_DTVB0_DVO0_ETSP_EPS1_ELFLR0_EMLL0_FSSC10_FL0_GLVWA2_GLVWB4_GRCGA1_GRCGB1_GRPM1_GRVWn1_GSU1_GSUASB_GLS0_ISA942_IU1_K1_KLA_LBSPPA0_LBSPPB1024_LPA0_LPB4_LDL1_LRVW4_LWPMn1_LDW0_FMA_MIAV0_MDA2_MO40_MMFSC_MKFGSU256_NTA0_NTB0_NTC0_NTD0_NEPBS0_NLCA2_NLCB2_ONLL1_OPLV0_PK0_PAP0_PGR2_PLR5_PKA0_SIA3_SLW1_SS1_SU8_SUM0_SUS256_SCIUI1_SPO1_SRVW0_SSO0_SVW2_SNLL0_TSGRA0_TSGRB0_TT4_128_TLDS0_UMLDSA0_UMLDSB0_U64SL1_USFGROn1_VAW1_VSn1_VW2_VWB4_VFLRP1_WSGRA0_WSGRB0_WS64_WG64_4_1_WGM1', 'dur': 292.752, 'custom_call_target': 'custom_call_target="__cudnn$convForward"', 'operands': ['bf16[1,16,32,60,104]{4,3,2,1,0}', 'bf16[5120,16,1,2,2]{4,3,2,1,0}'], 'outputs': 'NA', 'metadata': 'metadata={op_name="jit(forward_3d_conv)/jit(main)/conv_general_dilated" source_file="/workspace/conv-jax/jax_conv_profiling.py" source_line=77'}]</t>
         </is>
       </c>
+      <c r="M25" t="n">
+        <v>13.11999999987893</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -2257,6 +2315,9 @@
         <is>
           <t>[{'name': 'input_transpose_fusion', 'dur': 369.545, 'custom_call_target': 'NA', 'operands': ['bf16[1,5120,34,31,53]{4,3,2,1,0}'], 'outputs': 'NA', 'metadata': 'metadata={op_name="jit(forward_3d_conv)/jit(main)/conv_general_dilated" source_file="/workspace/conv-jax/jax_conv_profiling.py" source_line=77'}]</t>
         </is>
+      </c>
+      <c r="M26" t="n">
+        <v>295.7669999999925</v>
       </c>
     </row>
   </sheetData>
@@ -2957,7 +3018,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:N16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2973,108 +3034,938 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>total_direct_kernel_time_sum</t>
+          <t>UID</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Count</t>
+          <t>op category</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>total_direct_kernel_time_ms</t>
+          <t>total_direct_kernel_time</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Percentage (%)</t>
+          <t>direct_kernel_count</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Cumulative Percentage (%)</t>
+          <t>pid</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>time ms per gpu</t>
+          <t>tid</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Input Dims</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Input type</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Input Strides</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Concrete Inputs</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>kernel_details</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>GPU_kernel_launch_latency</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>total_input_bytes</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>input_transpose_fusion</t>
+          <t>loop_transpose_fusion</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1950.96</v>
-      </c>
-      <c r="C2" t="n">
-        <v>5</v>
+        <v>53</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Uncategorized Events/XLA</t>
+        </is>
       </c>
       <c r="D2" t="n">
-        <v>1.95096</v>
+        <v>6.89</v>
       </c>
       <c r="E2" t="n">
-        <v>95.32404242813051</v>
+        <v>1</v>
       </c>
       <c r="F2" t="n">
-        <v>95.32404242813051</v>
+        <v>8</v>
       </c>
       <c r="G2" t="n">
-        <v>1.95096</v>
+        <v>1</v>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>((1, 2, 2, 16, 5120),)</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>('bf16',)</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>()</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>()</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>[{'name': 'loop_transpose_fusion', 'dur': 6.89, 'custom_call_target': 'NA', 'operands': ['bf16[1,2,2,16,5120]{4,3,2,1,0}'], 'outputs': 'NA', 'metadata': 'metadata={op_name="kernel"'}]</t>
+        </is>
+      </c>
+      <c r="M2" t="n">
+        <v>20.94200000003912</v>
+      </c>
+      <c r="N2" t="n">
+        <v>655360</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>input_transpose_fusion_</t>
+          <t>input_transpose_fusion_1</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>69.261</v>
-      </c>
-      <c r="C3" t="n">
-        <v>5</v>
+        <v>54</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Uncategorized Events/XLA</t>
+        </is>
       </c>
       <c r="D3" t="n">
-        <v>0.06926099999999999</v>
+        <v>42.983</v>
       </c>
       <c r="E3" t="n">
-        <v>3.384097317533289</v>
+        <v>1</v>
       </c>
       <c r="F3" t="n">
-        <v>98.7081397456638</v>
+        <v>8</v>
       </c>
       <c r="G3" t="n">
-        <v>0.06926099999999999</v>
+        <v>1</v>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>((1, 32, 60, 104, 16),)</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>('bf16',)</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>()</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>()</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>[{'name': 'input_transpose_fusion_1', 'dur': 42.983, 'custom_call_target': 'NA', 'operands': ['bf16[1,32,60,104,16]{4,3,2,1,0}'], 'outputs': 'NA', 'metadata': 'metadata={op_name="x"'}]</t>
+        </is>
+      </c>
+      <c r="M3" t="n">
+        <v>12.1589999999851</v>
+      </c>
+      <c r="N3" t="n">
+        <v>6389760</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
+          <t>input_transpose_fusion</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>57</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Uncategorized Events/XLA</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>475.582</v>
+      </c>
+      <c r="E4" t="n">
+        <v>1</v>
+      </c>
+      <c r="F4" t="n">
+        <v>8</v>
+      </c>
+      <c r="G4" t="n">
+        <v>1</v>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>((1, 5120, 34, 31, 53),)</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>('bf16',)</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>()</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>()</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>[{'name': 'input_transpose_fusion', 'dur': 475.582, 'custom_call_target': 'NA', 'operands': ['bf16[1,5120,34,31,53]{4,3,2,1,0}'], 'outputs': 'NA', 'metadata': 'metadata={op_name="jit(forward_3d_conv)/jit(main)/conv_general_dilated" source_file="/workspace/conv-jax/jax_conv_profiling.py" source_line=77'}]</t>
+        </is>
+      </c>
+      <c r="M4" t="n">
+        <v>294.3659999999218</v>
+      </c>
+      <c r="N4" t="n">
+        <v>572026880</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
           <t>loop_transpose_fusion</t>
         </is>
       </c>
-      <c r="B4" t="n">
-        <v>26.44</v>
-      </c>
-      <c r="C4" t="n">
-        <v>5</v>
-      </c>
-      <c r="D4" t="n">
-        <v>0.02644</v>
-      </c>
-      <c r="E4" t="n">
-        <v>1.291860254336209</v>
-      </c>
-      <c r="F4" t="n">
-        <v>100</v>
-      </c>
-      <c r="G4" t="n">
-        <v>0.02644</v>
+      <c r="B5" t="n">
+        <v>58</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Uncategorized Events/XLA</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>5.048</v>
+      </c>
+      <c r="E5" t="n">
+        <v>1</v>
+      </c>
+      <c r="F5" t="n">
+        <v>8</v>
+      </c>
+      <c r="G5" t="n">
+        <v>1</v>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>((1, 2, 2, 16, 5120),)</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>('bf16',)</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>()</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>()</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>[{'name': 'loop_transpose_fusion', 'dur': 5.048, 'custom_call_target': 'NA', 'operands': ['bf16[1,2,2,16,5120]{4,3,2,1,0}'], 'outputs': 'NA', 'metadata': 'metadata={op_name="kernel"'}]</t>
+        </is>
+      </c>
+      <c r="M5" t="n">
+        <v>14.40200000000186</v>
+      </c>
+      <c r="N5" t="n">
+        <v>655360</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>input_transpose_fusion_1</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>59</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Uncategorized Events/XLA</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>6.689</v>
+      </c>
+      <c r="E6" t="n">
+        <v>1</v>
+      </c>
+      <c r="F6" t="n">
+        <v>8</v>
+      </c>
+      <c r="G6" t="n">
+        <v>1</v>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>((1, 32, 60, 104, 16),)</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>('bf16',)</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>()</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>()</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>[{'name': 'input_transpose_fusion_1', 'dur': 6.689, 'custom_call_target': 'NA', 'operands': ['bf16[1,32,60,104,16]{4,3,2,1,0}'], 'outputs': 'NA', 'metadata': 'metadata={op_name="x"'}]</t>
+        </is>
+      </c>
+      <c r="M6" t="n">
+        <v>10.92700000014156</v>
+      </c>
+      <c r="N6" t="n">
+        <v>6389760</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>input_transpose_fusion</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>62</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Uncategorized Events/XLA</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>366.06</v>
+      </c>
+      <c r="E7" t="n">
+        <v>1</v>
+      </c>
+      <c r="F7" t="n">
+        <v>8</v>
+      </c>
+      <c r="G7" t="n">
+        <v>1</v>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>((1, 5120, 34, 31, 53),)</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>('bf16',)</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>()</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>()</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>[{'name': 'input_transpose_fusion', 'dur': 366.06, 'custom_call_target': 'NA', 'operands': ['bf16[1,5120,34,31,53]{4,3,2,1,0}'], 'outputs': 'NA', 'metadata': 'metadata={op_name="jit(forward_3d_conv)/jit(main)/conv_general_dilated" source_file="/workspace/conv-jax/jax_conv_profiling.py" source_line=77'}]</t>
+        </is>
+      </c>
+      <c r="M7" t="n">
+        <v>295.3469999998342</v>
+      </c>
+      <c r="N7" t="n">
+        <v>572026880</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>loop_transpose_fusion</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>63</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Uncategorized Events/XLA</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>4.807</v>
+      </c>
+      <c r="E8" t="n">
+        <v>1</v>
+      </c>
+      <c r="F8" t="n">
+        <v>8</v>
+      </c>
+      <c r="G8" t="n">
+        <v>1</v>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>((1, 2, 2, 16, 5120),)</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>('bf16',)</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>()</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>()</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>[{'name': 'loop_transpose_fusion', 'dur': 4.807, 'custom_call_target': 'NA', 'operands': ['bf16[1,2,2,16,5120]{4,3,2,1,0}'], 'outputs': 'NA', 'metadata': 'metadata={op_name="kernel"'}]</t>
+        </is>
+      </c>
+      <c r="M8" t="n">
+        <v>14.72200000006706</v>
+      </c>
+      <c r="N8" t="n">
+        <v>655360</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>input_transpose_fusion_1</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>64</v>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Uncategorized Events/XLA</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>6.53</v>
+      </c>
+      <c r="E9" t="n">
+        <v>1</v>
+      </c>
+      <c r="F9" t="n">
+        <v>8</v>
+      </c>
+      <c r="G9" t="n">
+        <v>1</v>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>((1, 32, 60, 104, 16),)</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>('bf16',)</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>()</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>()</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>[{'name': 'input_transpose_fusion_1', 'dur': 6.53, 'custom_call_target': 'NA', 'operands': ['bf16[1,32,60,104,16]{4,3,2,1,0}'], 'outputs': 'NA', 'metadata': 'metadata={op_name="x"'}]</t>
+        </is>
+      </c>
+      <c r="M9" t="n">
+        <v>11.14699999988079</v>
+      </c>
+      <c r="N9" t="n">
+        <v>6389760</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>input_transpose_fusion</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>67</v>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Uncategorized Events/XLA</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>370.347</v>
+      </c>
+      <c r="E10" t="n">
+        <v>1</v>
+      </c>
+      <c r="F10" t="n">
+        <v>8</v>
+      </c>
+      <c r="G10" t="n">
+        <v>1</v>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>((1, 5120, 34, 31, 53),)</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>('bf16',)</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>()</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>()</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>[{'name': 'input_transpose_fusion', 'dur': 370.347, 'custom_call_target': 'NA', 'operands': ['bf16[1,5120,34,31,53]{4,3,2,1,0}'], 'outputs': 'NA', 'metadata': 'metadata={op_name="jit(forward_3d_conv)/jit(main)/conv_general_dilated" source_file="/workspace/conv-jax/jax_conv_profiling.py" source_line=77'}]</t>
+        </is>
+      </c>
+      <c r="M10" t="n">
+        <v>287.7750000001397</v>
+      </c>
+      <c r="N10" t="n">
+        <v>572026880</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>loop_transpose_fusion</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>68</v>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Uncategorized Events/XLA</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>4.968</v>
+      </c>
+      <c r="E11" t="n">
+        <v>1</v>
+      </c>
+      <c r="F11" t="n">
+        <v>8</v>
+      </c>
+      <c r="G11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>((1, 2, 2, 16, 5120),)</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>('bf16',)</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>()</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>()</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>[{'name': 'loop_transpose_fusion', 'dur': 4.968, 'custom_call_target': 'NA', 'operands': ['bf16[1,2,2,16,5120]{4,3,2,1,0}'], 'outputs': 'NA', 'metadata': 'metadata={op_name="kernel"'}]</t>
+        </is>
+      </c>
+      <c r="M11" t="n">
+        <v>21.33199999993667</v>
+      </c>
+      <c r="N11" t="n">
+        <v>655360</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>input_transpose_fusion_1</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>69</v>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Uncategorized Events/XLA</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>6.329</v>
+      </c>
+      <c r="E12" t="n">
+        <v>1</v>
+      </c>
+      <c r="F12" t="n">
+        <v>8</v>
+      </c>
+      <c r="G12" t="n">
+        <v>1</v>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>((1, 32, 60, 104, 16),)</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>('bf16',)</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>()</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>()</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>[{'name': 'input_transpose_fusion_1', 'dur': 6.329, 'custom_call_target': 'NA', 'operands': ['bf16[1,32,60,104,16]{4,3,2,1,0}'], 'outputs': 'NA', 'metadata': 'metadata={op_name="x"'}]</t>
+        </is>
+      </c>
+      <c r="M12" t="n">
+        <v>9.385000000009313</v>
+      </c>
+      <c r="N12" t="n">
+        <v>6389760</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>input_transpose_fusion</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>72</v>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Uncategorized Events/XLA</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>369.426</v>
+      </c>
+      <c r="E13" t="n">
+        <v>1</v>
+      </c>
+      <c r="F13" t="n">
+        <v>8</v>
+      </c>
+      <c r="G13" t="n">
+        <v>1</v>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>((1, 5120, 34, 31, 53),)</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>('bf16',)</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>()</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>()</t>
+        </is>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>[{'name': 'input_transpose_fusion', 'dur': 369.426, 'custom_call_target': 'NA', 'operands': ['bf16[1,5120,34,31,53]{4,3,2,1,0}'], 'outputs': 'NA', 'metadata': 'metadata={op_name="jit(forward_3d_conv)/jit(main)/conv_general_dilated" source_file="/workspace/conv-jax/jax_conv_profiling.py" source_line=77'}]</t>
+        </is>
+      </c>
+      <c r="M13" t="n">
+        <v>293.1029999998864</v>
+      </c>
+      <c r="N13" t="n">
+        <v>572026880</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>loop_transpose_fusion</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>73</v>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Uncategorized Events/XLA</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>4.727</v>
+      </c>
+      <c r="E14" t="n">
+        <v>1</v>
+      </c>
+      <c r="F14" t="n">
+        <v>8</v>
+      </c>
+      <c r="G14" t="n">
+        <v>1</v>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>((1, 2, 2, 16, 5120),)</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>('bf16',)</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>()</t>
+        </is>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>()</t>
+        </is>
+      </c>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>[{'name': 'loop_transpose_fusion', 'dur': 4.727, 'custom_call_target': 'NA', 'operands': ['bf16[1,2,2,16,5120]{4,3,2,1,0}'], 'outputs': 'NA', 'metadata': 'metadata={op_name="kernel"'}]</t>
+        </is>
+      </c>
+      <c r="M14" t="n">
+        <v>15.06200000015087</v>
+      </c>
+      <c r="N14" t="n">
+        <v>655360</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>input_transpose_fusion_1</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>74</v>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Uncategorized Events/XLA</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>6.73</v>
+      </c>
+      <c r="E15" t="n">
+        <v>1</v>
+      </c>
+      <c r="F15" t="n">
+        <v>8</v>
+      </c>
+      <c r="G15" t="n">
+        <v>1</v>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>((1, 32, 60, 104, 16),)</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>('bf16',)</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>()</t>
+        </is>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>()</t>
+        </is>
+      </c>
+      <c r="L15" t="inlineStr">
+        <is>
+          <t>[{'name': 'input_transpose_fusion_1', 'dur': 6.73, 'custom_call_target': 'NA', 'operands': ['bf16[1,32,60,104,16]{4,3,2,1,0}'], 'outputs': 'NA', 'metadata': 'metadata={op_name="x"'}]</t>
+        </is>
+      </c>
+      <c r="M15" t="n">
+        <v>11.5570000000298</v>
+      </c>
+      <c r="N15" t="n">
+        <v>6389760</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>input_transpose_fusion</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>77</v>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Uncategorized Events/XLA</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>369.545</v>
+      </c>
+      <c r="E16" t="n">
+        <v>1</v>
+      </c>
+      <c r="F16" t="n">
+        <v>8</v>
+      </c>
+      <c r="G16" t="n">
+        <v>1</v>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>((1, 5120, 34, 31, 53),)</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>('bf16',)</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>()</t>
+        </is>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>()</t>
+        </is>
+      </c>
+      <c r="L16" t="inlineStr">
+        <is>
+          <t>[{'name': 'input_transpose_fusion', 'dur': 369.545, 'custom_call_target': 'NA', 'operands': ['bf16[1,5120,34,31,53]{4,3,2,1,0}'], 'outputs': 'NA', 'metadata': 'metadata={op_name="jit(forward_3d_conv)/jit(main)/conv_general_dilated" source_file="/workspace/conv-jax/jax_conv_profiling.py" source_line=77'}]</t>
+        </is>
+      </c>
+      <c r="M16" t="n">
+        <v>295.7669999999925</v>
+      </c>
+      <c r="N16" t="n">
+        <v>572026880</v>
       </c>
     </row>
   </sheetData>
@@ -3088,14 +3979,127 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>total_direct_kernel_time_sum</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Count</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>total_direct_kernel_time_ms</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Percentage (%)</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Cumulative Percentage (%)</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>time ms per gpu</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>input_transpose_fusion</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>1950.96</v>
+      </c>
+      <c r="C2" t="n">
+        <v>5</v>
+      </c>
+      <c r="D2" t="n">
+        <v>1.95096</v>
+      </c>
+      <c r="E2" t="n">
+        <v>95.32404242813051</v>
+      </c>
+      <c r="F2" t="n">
+        <v>95.32404242813051</v>
+      </c>
+      <c r="G2" t="n">
+        <v>1.95096</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>input_transpose_fusion_</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>69.261</v>
+      </c>
+      <c r="C3" t="n">
+        <v>5</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.06926099999999999</v>
+      </c>
+      <c r="E3" t="n">
+        <v>3.384097317533289</v>
+      </c>
+      <c r="F3" t="n">
+        <v>98.7081397456638</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0.06926099999999999</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>loop_transpose_fusion</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>26.44</v>
+      </c>
+      <c r="C4" t="n">
+        <v>5</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.02644</v>
+      </c>
+      <c r="E4" t="n">
+        <v>1.291860254336209</v>
+      </c>
+      <c r="F4" t="n">
+        <v>100</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0.02644</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -3302,14 +4306,20 @@
           <t>(1, 5120, 34, 31, 53)</t>
         </is>
       </c>
-      <c r="F2" t="b">
-        <v>0</v>
-      </c>
-      <c r="G2" t="n">
-        <v>2</v>
-      </c>
-      <c r="H2" t="b">
-        <v>0</v>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
       </c>
       <c r="I2" t="n">
         <v>2.28810752</v>
@@ -3416,14 +4426,20 @@
           <t>(1, 5120, 34, 31, 53)</t>
         </is>
       </c>
-      <c r="F3" t="b">
-        <v>0</v>
-      </c>
-      <c r="G3" t="n">
-        <v>2</v>
-      </c>
-      <c r="H3" t="b">
-        <v>0</v>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
       </c>
       <c r="I3" t="n">
         <v>2.28810752</v>

</xml_diff>